<commit_message>
Port map template minor fixes
Added secondary functions for RPI pinouts
Added secondary functions for analog ports
</commit_message>
<xml_diff>
--- a/doc/Template-PortMapping.xlsx
+++ b/doc/Template-PortMapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uq-my.sharepoint.com/personal/uqltan14_uq_edu_au/Documents/Civil/Data_logger/hardware-datalogger/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{421E843E-B4AB-4636-AAE0-2C89A54FF965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{157C8D5D-FD47-4153-81B0-0CF9D5FCA495}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{6D1081D1-DE6D-410F-9B55-CDE76CF5AA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38955256-FC53-4459-8C69-8362914598FD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="64">
   <si>
     <t>POWER</t>
   </si>
@@ -57,12 +57,6 @@
     <t>RPI IO</t>
   </si>
   <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>RX</t>
-  </si>
-  <si>
     <t>RPI Switch</t>
   </si>
   <si>
@@ -132,12 +126,6 @@
     <t>A14 (68, SDI12)</t>
   </si>
   <si>
-    <t>A15 (69, Vsense, SDI12)</t>
-  </si>
-  <si>
-    <t>A0 (54, DHT22)</t>
-  </si>
-  <si>
     <t>12V</t>
   </si>
   <si>
@@ -177,22 +165,67 @@
     <t>Rx3 (15)</t>
   </si>
   <si>
-    <t>SC (20)</t>
-  </si>
-  <si>
-    <t>SD (21)</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>&lt;Datalogger Hostname&gt;</t>
   </si>
   <si>
-    <t>13 (Soft Rx)</t>
-  </si>
-  <si>
-    <t>16 (Soft Rx)</t>
+    <t>8 (5V/12V)</t>
+  </si>
+  <si>
+    <t>10 (Reverse 5V/12V)</t>
+  </si>
+  <si>
+    <t>11 (Reverse 5V/12V)</t>
+  </si>
+  <si>
+    <t>12 (Reverse 5V/12V)</t>
+  </si>
+  <si>
+    <t>13 (Reverse 5V/12V)</t>
+  </si>
+  <si>
+    <t>SC (I2C MUX**, 20)</t>
+  </si>
+  <si>
+    <t>SD (I2C MUX**, 21)</t>
+  </si>
+  <si>
+    <t>A0 (54, DHT22**)</t>
+  </si>
+  <si>
+    <t>A15 (69, Vsense*, SDI12)</t>
+  </si>
+  <si>
+    <t>9 (5V/12V, Vsense*)</t>
+  </si>
+  <si>
+    <t>TX** (14)</t>
+  </si>
+  <si>
+    <t>RX** (15)</t>
+  </si>
+  <si>
+    <t>10 (MOSI)</t>
+  </si>
+  <si>
+    <t>2 (SDA)</t>
+  </si>
+  <si>
+    <t>11 (SCK)</t>
+  </si>
+  <si>
+    <t>3 (SCL)</t>
+  </si>
+  <si>
+    <t>9 (MISO)</t>
+  </si>
+  <si>
+    <t>13 (Soft Rx*)</t>
+  </si>
+  <si>
+    <t>16 (Soft Rx*)</t>
   </si>
 </sst>
 </file>
@@ -253,7 +286,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -276,11 +309,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,9 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -330,6 +389,31 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,211 +710,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="A1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>39</v>
+      <c r="H2" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="16"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="16"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="16"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="16"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="16"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="16"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="16"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="16"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="16"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="16"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="16"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="19"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
@@ -917,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4034BC67-5EBE-4A9D-A470-527DEEA560E7}">
-  <dimension ref="A1:B138"/>
+  <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,978 +1016,994 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>2</v>
+      <c r="A2" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>10</v>
-      </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>11</v>
+      <c r="A6" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>7</v>
+      <c r="A7" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>21</v>
+      <c r="A10" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>18</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>8</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>12</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="8">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="7"/>
+      <c r="A21" s="8">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>25</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
-        <v>26</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7"/>
+      <c r="A31" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>37</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A46" s="26"/>
+      <c r="B46" s="27"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A47" s="21"/>
+      <c r="B47" s="22"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="22"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="22"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="29"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B51" s="7"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
-        <v>0</v>
+      <c r="A52" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="8">
-        <v>1</v>
+      <c r="A53" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
-        <v>2</v>
+      <c r="A54" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="8">
-        <v>3</v>
+      <c r="A55" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="8">
-        <v>4</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A56" s="30"/>
+      <c r="B56" s="27"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="8">
-        <v>5</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A57" s="31"/>
+      <c r="B57" s="29"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
-        <v>6</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A58" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="8">
-        <v>7</v>
+      <c r="A59" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
-      <c r="B60" s="7"/>
+      <c r="A60" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" s="7"/>
+      <c r="A61" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="8">
+        <v>22</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
+        <v>23</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="8">
+        <v>24</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
+        <v>25</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="8">
+        <v>26</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="8">
+        <v>27</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
+        <v>28</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="8">
+        <v>29</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="8">
+        <v>30</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="8">
+        <v>31</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="8">
+        <v>32</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="8">
+        <v>33</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="8">
+        <v>34</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="8">
+        <v>35</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="8">
+        <v>36</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="8">
+        <v>37</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="8">
+        <v>38</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="8">
+        <v>39</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="8">
+        <v>40</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="8">
+        <v>41</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="8">
+        <v>42</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="8">
         <v>43</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+      <c r="B86" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="8">
         <v>44</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
+      <c r="B87" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
         <v>45</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
+      <c r="B88" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="8">
         <v>46</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+      <c r="B89" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="8">
         <v>47</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
+      <c r="B90" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="8">
         <v>48</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B70" s="7"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
-      <c r="B78" s="7"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B79" s="7"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="7"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
-      <c r="B85" s="7"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="7"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
-      <c r="B87" s="7"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
-      <c r="B88" s="7"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
-      <c r="B89" s="7"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
-      <c r="B90" s="7"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
-      <c r="B91" s="7"/>
+      <c r="B91" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
-      <c r="B92" s="7"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="9"/>
-      <c r="B93" s="7"/>
+      <c r="A92" s="8">
+        <v>49</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
-      <c r="B94" s="7"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="9"/>
-      <c r="B95" s="7"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="9"/>
-      <c r="B96" s="7"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="9"/>
-      <c r="B97" s="7"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
-      <c r="B98" s="7"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="9"/>
-      <c r="B99" s="7"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="9"/>
-      <c r="B100" s="7"/>
+      <c r="A94" s="5"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="9"/>
+      <c r="A101" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="B101" s="7"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B102" s="7"/>
+      <c r="A102" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="8">
-        <v>9</v>
+      <c r="A104" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="8">
-        <v>10</v>
+      <c r="A105" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="8">
-        <v>12</v>
+      <c r="A107" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="8">
-        <v>13</v>
+      <c r="A108" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="8">
-        <v>23</v>
+      <c r="A110" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="8">
-        <v>25</v>
+      <c r="A112" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="8">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="8">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="8">
-        <v>30</v>
+      <c r="A117" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="8">
-        <v>31</v>
+      <c r="A118" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="8">
-        <v>32</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A119" s="24"/>
+      <c r="B119" s="25"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="8">
-        <v>33</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A120" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" s="7"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="8">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="8">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="8">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="8">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="8">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="8">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="8">
-        <v>42</v>
-      </c>
-      <c r="B129" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A129" s="21"/>
+      <c r="B129" s="22"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="8">
-        <v>43</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A130" s="21"/>
+      <c r="B130" s="22"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="8">
-        <v>44</v>
-      </c>
-      <c r="B131" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A131" s="21"/>
+      <c r="B131" s="22"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="8">
-        <v>45</v>
-      </c>
-      <c r="B132" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A132" s="21"/>
+      <c r="B132" s="22"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="8">
-        <v>46</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A133" s="21"/>
+      <c r="B133" s="22"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="8">
-        <v>47</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A134" s="21"/>
+      <c r="B134" s="22"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="8">
-        <v>48</v>
-      </c>
-      <c r="B135" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A135" s="21"/>
+      <c r="B135" s="22"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="8">
-        <v>49</v>
-      </c>
-      <c r="B136" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A136" s="21"/>
+      <c r="B136" s="22"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="21"/>
+      <c r="B137" s="22"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="5"/>
+      <c r="A138" s="21"/>
+      <c r="B138" s="22"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="21"/>
+      <c r="B139" s="22"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="21"/>
+      <c r="B140" s="22"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="21"/>
+      <c r="B141" s="22"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="21"/>
+      <c r="B142" s="22"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="21"/>
+      <c r="B143" s="22"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="21"/>
+      <c r="B144" s="22"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="21"/>
+      <c r="B145" s="22"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="21"/>
+      <c r="B146" s="22"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="21"/>
+      <c r="B147" s="22"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="21"/>
+      <c r="B148" s="22"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="23"/>
+      <c r="B149" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>